<commit_message>
Added results for 8-4
</commit_message>
<xml_diff>
--- a/resultados/resultados_8-2.xlsx
+++ b/resultados/resultados_8-2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Eduardo Gaitán</t>
+          <t>Roberto Zúñiga</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>68169</v>
+        <v>40788</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -486,12 +486,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Luis Duke</t>
+          <t>Jorge Bloise Iglesias</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TipoDeSeleccion.COCIENTE</t>
+          <t>TipoDeSeleccion.RESIDUO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>66324</v>
+        <v>40205</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -509,21 +509,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Alexandra Brenes</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>TipoDeSeleccion.COCIENTE</t>
-        </is>
-      </c>
+          <t>Cristal A Balabarca Cedeño</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>LP2</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>65103</v>
+        <v>39640</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -532,21 +528,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Doctora Yarelis Rodríguez</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>TipoDeSeleccion.RESIDUO</t>
-        </is>
-      </c>
+          <t>Juan Carlos Rojas Barrios</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>LP2</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>64498</v>
+        <v>38653</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -555,7 +547,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ángel Ortega González</t>
+          <t>Eulogio Castillo Marín</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -565,7 +557,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>64280</v>
+        <v>38176</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -574,17 +566,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Felipe Chong</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>Doctor Ernesto Cedeño</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TipoDeSeleccion.MEDIOCOCIENTE</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LP2</t>
+          <t>MOCA</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>63912</v>
+        <v>14577</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -593,17 +589,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Francisco Garcés</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>Grace Hernández</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TipoDeSeleccion.RESIDUO</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>LP2</t>
+          <t>MOCA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>63166</v>
+        <v>12697</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -612,21 +612,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Luis Eduardo Camacho</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>TipoDeSeleccion.COCIENTE</t>
-        </is>
-      </c>
+          <t>Mark Harrick Atie</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>MOCA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>19267</v>
+        <v>11921</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -635,21 +631,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Omar Ortega</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>TipoDeSeleccion.RESIDUO</t>
-        </is>
-      </c>
+          <t>Gabriel Menasche</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>MOCA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>17705</v>
+        <v>11684</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -658,17 +650,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Justiniani Miguel</t>
+          <t>Javier Eduardo Baldeolivar</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>MOCA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>16126</v>
+        <v>11541</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -677,17 +669,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dalia Bernal</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+          <t>Javier Sucre</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TipoDeSeleccion.MEDIOCOCIENTE</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>PRD</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>15890</v>
+        <v>10441</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -696,21 +692,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Raúl Pineda</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>TipoDeSeleccion.MEDIOCOCIENTE</t>
-        </is>
-      </c>
+          <t>Doctor Víctor Castillo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
           <t>PRD</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>15730</v>
+        <v>9393</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -719,45 +711,45 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Profesora Dalila Mosquera</t>
+          <t>Charlie Sousa-Lennox</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ALIANZA</t>
+          <t>PRD</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>15558</v>
+        <v>9095</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Marcos González</t>
+          <t>Josi El Bukele</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>MOLIRENA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>15496</v>
+        <v>8621</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Gerald Cumberbatch</t>
+          <t>Alejandro Perez</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -767,7 +759,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>15200</v>
+        <v>8282</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -776,36 +768,36 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>José Ruiloba</t>
+          <t>Helmut de Puy</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PRD</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>13566</v>
+        <v>8104</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Luis Oliva</t>
+          <t>Dra Nitzia Torres</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PRD</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>12045</v>
+        <v>7961</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -814,17 +806,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Zulay Rodríguez Lu</t>
+          <t>César Zapata Muñoz</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>LP1</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>11161</v>
+        <v>7532</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -833,26 +825,26 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pancho Alemán</t>
+          <t>Gilberto Romero</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MOLIRENA</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9857</v>
+        <v>7337</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Leandro Ávila</t>
+          <t>Guapo López</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -862,7 +854,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9071</v>
+        <v>6271</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -871,17 +863,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Kathy Ramos</t>
+          <t>Raúl Fernández</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PRD</t>
+          <t>LP3</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>7483</v>
+        <v>4230</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -890,26 +882,26 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Calixto Silgado</t>
+          <t>Albertito Guerra</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PRD</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6647</v>
+        <v>4099</v>
       </c>
       <c r="E23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Arnulfo González</t>
+          <t>Yadelis González</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -919,7 +911,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>6533</v>
+        <v>3815</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -928,17 +920,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Liney Mena</t>
+          <t>Daniel Lombana</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LP1</t>
+          <t>LP3</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>6448</v>
+        <v>3194</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -947,17 +939,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>José Luis Blandón</t>
+          <t>Omar Elías Castillo López</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LP1</t>
+          <t>POPULAR</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>6114</v>
+        <v>3160</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -966,17 +958,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ricardo Vásquez Ambientalista</t>
+          <t>Delbys Holmes de Richa</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LP1</t>
+          <t>LP3</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>6090</v>
+        <v>3127</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -985,17 +977,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Cesar Caicedo</t>
+          <t>Fulo Linares</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>6033</v>
+        <v>2629</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1004,17 +996,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>José Caballero</t>
+          <t>Dr Herick Bernal</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>LP1</t>
+          <t>POPULAR</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>5986</v>
+        <v>2603</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1023,17 +1015,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Yahaira Perén de Toureau</t>
+          <t>Ariel Lim Yueng</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MOCA</t>
+          <t>POPULAR</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>4936</v>
+        <v>2495</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1042,17 +1034,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Dempsil del Rosario Arroyo</t>
+          <t>Alex Charles</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MOCA</t>
+          <t>POPULAR</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>4889</v>
+        <v>2362</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1061,7 +1053,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Itzi Atencio</t>
+          <t>Sebastian Abadía</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1071,26 +1063,26 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4856</v>
+        <v>2212</v>
       </c>
       <c r="E32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ricardo Antonio Córtes Bonilla</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MOCA</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4694</v>
+        <v>1953</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1099,17 +1091,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Roy Jiménez</t>
+          <t>Stephanie Cardoze</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MOCA</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4692</v>
+        <v>1841</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1118,17 +1110,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Alcibiades Al Méndez Cabrera</t>
+          <t>Miguel Gallardo Ferrer</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MOCA</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>4667</v>
+        <v>1840</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1137,17 +1129,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Eric Portocarrero</t>
+          <t>Ramiro López</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3397</v>
+        <v>1683</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1156,17 +1148,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Félix Moulanier</t>
+          <t>Chris Herrera</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>POPULAR</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>3255</v>
+        <v>1619</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1175,17 +1167,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Jean Marcel Chery Periodista</t>
+          <t>Bebito C</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>LP3</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3174</v>
+        <v>1593</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1194,17 +1186,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Jacky Hurtado Payne</t>
+          <t>Carmen Nadine Barrios</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>POPULAR</t>
+          <t>MOLIRENA</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2862</v>
+        <v>1285</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1213,17 +1205,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Abraham Martinez</t>
+          <t>Ricardo Alvarado</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>PAIS</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>2843</v>
+        <v>470</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1232,17 +1224,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Jayro García</t>
+          <t>Elizabeth Acosta</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LP3</t>
+          <t>PAIS</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2841</v>
+        <v>469</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1251,17 +1243,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sugey Tatiana Rueda</t>
+          <t>Raúl Ricardo Rodríguez</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>LP3</t>
+          <t>PAIS</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>2724</v>
+        <v>407</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1270,17 +1262,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Jorge Simons Jr.</t>
+          <t>Otoniel García</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>POPULAR</t>
+          <t>ALIANZA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>2636</v>
+        <v>406</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1289,17 +1281,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Nitzeira Watson</t>
+          <t>Iván Montalvo</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>POPULAR</t>
+          <t>PAIS</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2544</v>
+        <v>362</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -1308,551 +1300,19 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Machuca José</t>
+          <t>Lital Smith</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>POPULAR</t>
+          <t>PAIS</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2483</v>
+        <v>350</v>
       </c>
       <c r="E45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Victor Córdoba</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>2383</v>
-      </c>
-      <c r="E46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Carlos Melgar</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>2225</v>
-      </c>
-      <c r="E47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Ariette Paredes</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>MOLIRENA</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>2142</v>
-      </c>
-      <c r="E48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Roberto Nieto</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>PAN</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>2136</v>
-      </c>
-      <c r="E49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Victor Díaz</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>CD</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>2083</v>
-      </c>
-      <c r="E50" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Nadgee Bonilla</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>PAN</t>
-        </is>
-      </c>
-      <c r="D51" t="n">
-        <v>1987</v>
-      </c>
-      <c r="E51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Cleyder Guevara</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>MOLIRENA</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>1912</v>
-      </c>
-      <c r="E52" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Carlos "DJ Cuca" Rivera</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>MOLIRENA</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>1814</v>
-      </c>
-      <c r="E53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>El Vecino</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>MOLIRENA</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>1776</v>
-      </c>
-      <c r="E54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Orlando Aguilar</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>MOLIRENA</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>1724</v>
-      </c>
-      <c r="E55" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Enrique Marin</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>PAN</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>1700</v>
-      </c>
-      <c r="E56" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Silka Sánchez de González</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>PAIS</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>1608</v>
-      </c>
-      <c r="E57" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Mario Prado</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>PAN</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>1592</v>
-      </c>
-      <c r="E58" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Jorge Alvarado</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>PAN</t>
-        </is>
-      </c>
-      <c r="D59" t="n">
-        <v>1591</v>
-      </c>
-      <c r="E59" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Pablo Castilla</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>PAN</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
-        <v>1537</v>
-      </c>
-      <c r="E60" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Christian Toto Castillo</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>MOLIRENA</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>1374</v>
-      </c>
-      <c r="E61" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Rudelda Guzmán</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>PAIS</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>1301</v>
-      </c>
-      <c r="E62" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Sergio Bairnals</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>PAIS</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>1013</v>
-      </c>
-      <c r="E63" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Javier Montenegro</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>PAIS</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>934</v>
-      </c>
-      <c r="E64" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Manuel Landero Herrera</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>PAIS</t>
-        </is>
-      </c>
-      <c r="D65" t="n">
-        <v>915</v>
-      </c>
-      <c r="E65" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Vicente Torres Ramos</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>PAIS</t>
-        </is>
-      </c>
-      <c r="D66" t="n">
-        <v>906</v>
-      </c>
-      <c r="E66" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Toto</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>PAIS</t>
-        </is>
-      </c>
-      <c r="D67" t="n">
-        <v>851</v>
-      </c>
-      <c r="E67" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Juan Antonio Tejada Pinillo</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>ALIANZA</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>725</v>
-      </c>
-      <c r="E68" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Jovanita de Roa</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>ALIANZA</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>696</v>
-      </c>
-      <c r="E69" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Luis Romero</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>ALIANZA</t>
-        </is>
-      </c>
-      <c r="D70" t="n">
-        <v>688</v>
-      </c>
-      <c r="E70" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Fernando Samaniego</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>ALIANZA</t>
-        </is>
-      </c>
-      <c r="D71" t="n">
-        <v>687</v>
-      </c>
-      <c r="E71" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Raúl Patiño</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>ALIANZA</t>
-        </is>
-      </c>
-      <c r="D72" t="n">
-        <v>674</v>
-      </c>
-      <c r="E72" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Ricauter Sinisterra Castillo</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>ALIANZA</t>
-        </is>
-      </c>
-      <c r="D73" t="n">
-        <v>646</v>
-      </c>
-      <c r="E73" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>